<commit_message>
domestic update and user data
</commit_message>
<xml_diff>
--- a/user-data/ethiopia-nigeria-r7/ethiopia-nigeria-r7.xlsx
+++ b/user-data/ethiopia-nigeria-r7/ethiopia-nigeria-r7.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Nigeria</t>
+  </si>
+  <si>
+    <t> </t>
   </si>
   <si>
     <t>Name: ethiopia-nigeria-r7</t>
@@ -406,72 +409,72 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -991,6 +994,15 @@
         <v>0.005013617</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>